<commit_message>
some edits to docs files and Rules
</commit_message>
<xml_diff>
--- a/tweets.xlsx
+++ b/tweets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Semantic\hate_tweet_map\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alessia\Documents\GitHub\hate_tweet_map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08C78A78-2475-45E0-8648-330CEB05D746}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C2EDB8-6DD3-470E-B05B-1CBBFC9AB3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tweets" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="86">
   <si>
     <t>Tweet</t>
   </si>
@@ -40,9 +40,6 @@
     <t>Il Covid deve aver avuto conseguenze pesanti sul cervello di certi magistrati.</t>
   </si>
   <si>
-    <t>Lavoratori della mia Patria, ho fede nel Cile e nel suo destino. Altri uomini supereranno questo momento grigio e amaro in cui il tradimento pretende di imporsi.	0.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">Di Maio,Italia difende diritti, come in casi Regeni e Zaki </t>
   </si>
   <si>
@@ -58,7 +55,7 @@
     <t>Lettori e lettrici del Corriere della Sera, affrettatevi! Due volumi a soli 3 euro!</t>
   </si>
   <si>
-    <t>0.5</t>
+    <t>0.25</t>
   </si>
   <si>
     <t>La riunione ha visto consiglieri e consigliere comunali discutere del rincaro sulle bollette.</t>
@@ -67,7 +64,7 @@
     <t>Gli scrittori e le scrittrici iscritti al concorso sono invitati/e a consegnare il manoscritto entro le ore 00.00 del giorno 3 gennaio.</t>
   </si>
   <si>
-    <t>0.6</t>
+    <t>0.35</t>
   </si>
   <si>
     <t>le insegnanti e gli insegnanti devono reagire alla mancanza totale di sicurezza e al trattamento riservato come lavoratori e lavoratrici schiavi e senza diritto alla salute, pur di tenere aperta la scuola, dove ricordo nulla è stato fatto in questi anni.</t>
@@ -94,111 +91,111 @@
     <t>Putin e la Merkel sono andati a comprare un kg di marijuana</t>
   </si>
   <si>
+    <t xml:space="preserve">Anche la cancelliera si arrende al grande bluff, che non é il virus intendiamoci subito che purtroppo esiste e provoca danni a persone con già problemi., ma la psicosi e tutto il castello dietro per cui chiudere é l unica soluzione </t>
+  </si>
+  <si>
+    <t>I lottatori di sumo sono degli uomini possenti, le lottatrici di sumo sono solo ciccione.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> margaret thatcher  è stata primo ministro del regno unito dal maggio 1979 al  novembre 1990...e non c'erano le quote rosa. </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'merito della misura per i non vaccinati introdotta il 2 dicembre dalla cancelliera uscente angela merkel' </t>
+  </si>
+  <si>
+    <t>Una donna al Quirinale nel rispetto dei colori dell’arcobaleno, non del rosa</t>
+  </si>
+  <si>
+    <t>Il sindaco donna Simona Laurito ha pubblicato un emendamento riguardo il DPCM del marzo 2020.</t>
+  </si>
+  <si>
+    <t>La donna cannone è una canzone di Francesco De Gregori.</t>
+  </si>
+  <si>
+    <t>Giuseppe e Nicola sono due magistrati di grande successo.</t>
+  </si>
+  <si>
+    <t>Pace agli uomini di buona volontà.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Il/la signor/a Bentivoglio si rivolga all'amministratore di condominio per informazioni </t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arbitro. Personalmente lo preferisco. Come preferisco sindaco a sindaca. 90% quando mi dicono arbitra è per sottolineare che sono una donna. Credo che quando non ci sarà più l’esigenza di sottolinearlo, allora vorrà dire che ci sarà davvero parità. </t>
+  </si>
+  <si>
+    <t>La Raggi ha stilato una lista di regole da rispettare nei weekend.</t>
+  </si>
+  <si>
+    <t>L'uomo di Altamura è considerato una fra le più grandi scoperte in Puglia</t>
+  </si>
+  <si>
+    <t>Questi uomini di merda...@nicolapanino</t>
+  </si>
+  <si>
+    <t>Gli avvocati sono la rovina della società</t>
+  </si>
+  <si>
+    <t>Il giudice Giovanni Falcone è stato un esempio per la Giustizia Italiana.</t>
+  </si>
+  <si>
+    <t>Il miracolo che salva il mondo dalla sua naturale rovina è la nascita di uomini nuovi..., la nascita di quella fede e speranza... che hanno trovato la loro più succinta e gioiosa espressione in una piccola frase dei Vangeli: "Ecco vi è nato un bambino".</t>
+  </si>
+  <si>
+    <t>Ma il tampone per andare al cinema deve pagarlo l'uomo o la donna?</t>
+  </si>
+  <si>
+    <t>Daniela Grassi è un avvocato formidabile</t>
+  </si>
+  <si>
+    <t>@ceciliadelia @repubblica Non una donna candidata a sindaco due mesi fa, la proposta di candidarsi fatta a Conte per primo e adesso a sventolare la priorità dell'uguaglianza di genere. Credibile</t>
+  </si>
+  <si>
+    <t>Maria Dolores cerca un/una addetto/a alla pulizia dei bagni.</t>
+  </si>
+  <si>
+    <t>Il razzismo è solo negli occhi di chi guarda. Viva le lavoratrici e i lavoratori perbene!</t>
+  </si>
+  <si>
+    <t>Buona #SantaBarbara agli Uomini e alle Donne del Corpo dei Vigili del Fuoco! E grazie per quello che fate ogni giorno rischiando la vita per salvare quella degli altri.</t>
+  </si>
+  <si>
+    <t>E se chi sostiene che lei/lui se la sia andata a cercare, fosse egli/ella stesso/a che se le sta andando a cercare?</t>
+  </si>
+  <si>
+    <t>flexatemi il/la vostr* miglior amic*	0.25</t>
+  </si>
+  <si>
+    <t>Il PD annuncia che candiderà nel collegio di Roma-Trionfale Cecilia D'Elia. A poche ore dalla scadenza si aspetta ancora di conoscere il/la candidato/a di cdx.</t>
+  </si>
+  <si>
+    <t>Eh niente Peril e Engin, hanno lasciato l’art life per fare gli avvocati.</t>
+  </si>
+  <si>
+    <t>Una volta i magistrati parlavano con le sentenze, oggi sono presenti nel mondo pubblico e politico e quindi distruggono la loro imparzialità.</t>
+  </si>
+  <si>
+    <t>La capacità di applicare l'intelligenza e il talento sul piano pratico e teorico determinano l'ingegno dell'uomo.	-0.25</t>
+  </si>
+  <si>
+    <t>Vorrei ricordare agli uomini di scarsa memoria, e ai virologi con un po' di sale in zucca,</t>
+  </si>
+  <si>
+    <t>Gli uomini politici sono uguali dappertutto. Promettono di costruire un ponte anche dove non c’è un fiume. (Nikita Chrušcëv)</t>
+  </si>
+  <si>
+    <t>Grazie alle donne e agli uomini di #ItaliaViva grazie a #MatteoRenzi</t>
+  </si>
+  <si>
+    <t>La donna avvocato si rifiuta di difendere l' uxoricida. Un contrasto insostenibile con il suo impegno in difesa delle donne vittime di violenza</t>
+  </si>
+  <si>
     <t>-0.5</t>
   </si>
   <si>
-    <t xml:space="preserve">Anche la cancelliera si arrende al grande bluff, che non é il virus intendiamoci subito che purtroppo esiste e provoca danni a persone con già problemi., ma la psicosi e tutto il castello dietro per cui chiudere é l unica soluzione </t>
-  </si>
-  <si>
-    <t>I lottatori di sumo sono degli uomini possenti, le lottatrici di sumo sono solo ciccione.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> margaret thatcher  è stata primo ministro del regno unito dal maggio 1979 al  novembre 1990...e non c'erano le quote rosa. </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 'merito della misura per i non vaccinati introdotta il 2 dicembre dalla cancelliera uscente angela merkel' </t>
-  </si>
-  <si>
-    <t>Una donna al Quirinale nel rispetto dei colori dell’arcobaleno, non del rosa</t>
-  </si>
-  <si>
-    <t>Il sindaco donna Simona Laurito ha pubblicato un emendamento riguardo il DPCM del marzo 2020.</t>
-  </si>
-  <si>
-    <t>La donna cannone è una canzone di Francesco De Gregori.</t>
-  </si>
-  <si>
-    <t>Giuseppe e Nicola sono due magistrati di grande successo.</t>
-  </si>
-  <si>
-    <t>Pace agli uomini di buona volontà.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Il/la signor/a Bentivoglio si rivolga all'amministratore di condominio per informazioni </t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arbitro. Personalmente lo preferisco. Come preferisco sindaco a sindaca. 90% quando mi dicono arbitra è per sottolineare che sono una donna. Credo che quando non ci sarà più l’esigenza di sottolinearlo, allora vorrà dire che ci sarà davvero parità. </t>
-  </si>
-  <si>
-    <t>La Raggi ha stilato una lista di regole da rispettare nei weekend.</t>
-  </si>
-  <si>
-    <t>L'uomo di Altamura è considerato una fra le più grandi scoperte in Puglia</t>
-  </si>
-  <si>
-    <t>Questi uomini di merda...@nicolapanino</t>
-  </si>
-  <si>
-    <t>Gli avvocati sono la rovina della società</t>
-  </si>
-  <si>
-    <t>Il giudice Giovanni Falcone è stato un esempio per la Giustizia Italiana.</t>
-  </si>
-  <si>
-    <t>Il miracolo che salva il mondo dalla sua naturale rovina è la nascita di uomini nuovi..., la nascita di quella fede e speranza... che hanno trovato la loro più succinta e gioiosa espressione in una piccola frase dei Vangeli: "Ecco vi è nato un bambino".</t>
-  </si>
-  <si>
-    <t>Ma il tampone per andare al cinema deve pagarlo l'uomo o la donna?</t>
-  </si>
-  <si>
-    <t>Daniela Grassi è un avvocato formidabile</t>
-  </si>
-  <si>
-    <t>@ceciliadelia @repubblica Non una donna candidata a sindaco due mesi fa, la proposta di candidarsi fatta a Conte per primo e adesso a sventolare la priorità dell'uguaglianza di genere. Credibile</t>
-  </si>
-  <si>
-    <t>Maria Dolores cerca un/una addetto/a alla pulizia dei bagni.</t>
-  </si>
-  <si>
-    <t>Il razzismo è solo negli occhi di chi guarda. Viva le lavoratrici e i lavoratori perbene!</t>
-  </si>
-  <si>
-    <t>Buona #SantaBarbara agli Uomini e alle Donne del Corpo dei Vigili del Fuoco! E grazie per quello che fate ogni giorno rischiando la vita per salvare quella degli altri.</t>
-  </si>
-  <si>
-    <t>E se chi sostiene che lei/lui se la sia andata a cercare, fosse egli/ella stesso/a che se le sta andando a cercare?</t>
-  </si>
-  <si>
-    <t>flexatemi il/la vostr* miglior amic*	0.25</t>
-  </si>
-  <si>
-    <t>Il PD annuncia che candiderà nel collegio di Roma-Trionfale Cecilia D'Elia. A poche ore dalla scadenza si aspetta ancora di conoscere il/la candidato/a di cdx.</t>
-  </si>
-  <si>
-    <t>Eh niente Peril e Engin, hanno lasciato l’art life per fare gli avvocati.</t>
-  </si>
-  <si>
-    <t>Una volta i magistrati parlavano con le sentenze, oggi sono presenti nel mondo pubblico e politico e quindi distruggono la loro imparzialità.</t>
-  </si>
-  <si>
-    <t>La capacità di applicare l'intelligenza e il talento sul piano pratico e teorico determinano l'ingegno dell'uomo.	-0.25</t>
-  </si>
-  <si>
-    <t>Vorrei ricordare agli uomini di scarsa memoria, e ai virologi con un po' di sale in zucca,</t>
-  </si>
-  <si>
-    <t>Gli uomini politici sono uguali dappertutto. Promettono di costruire un ponte anche dove non c’è un fiume. (Nikita Chrušcëv)</t>
-  </si>
-  <si>
-    <t>Grazie alle donne e agli uomini di #ItaliaViva grazie a #MatteoRenzi</t>
-  </si>
-  <si>
-    <t>La donna avvocato si rifiuta di difendere l' uxoricida. Un contrasto insostenibile con il suo impegno in difesa delle donne vittime di violenza</t>
-  </si>
-  <si>
     <t xml:space="preserve">#donciotti rappresenta gli uomini di chiesa che rispetto! </t>
   </si>
   <si>
@@ -230,12 +227,63 @@
   </si>
   <si>
     <t>Perché i magistrati non vengono mai puniti, quando sono colpevoli? Perché sono al di sopra della legge?? Sta storia deve finire!!"</t>
+  </si>
+  <si>
+    <t>ground_truth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lavoratori della mia Patria, ho fede nel Cile e nel suo destino. Altri uomini supereranno questo momento grigio e amaro in cui il tradimento pretende di imporsi.	</t>
+  </si>
+  <si>
+    <t>ambiguità di linguaggio, non risolvibile</t>
+  </si>
+  <si>
+    <t>Lavoratori con la maiuscola non viene letto correttamente</t>
+  </si>
+  <si>
+    <t>Il pattern deve essere checkato per l'esistenza o per quante volte viene trovato?</t>
+  </si>
+  <si>
+    <t>In realtà dovrebbe essere triggerata anche la regola che vede che ci sia solo il plurale maschile, ma non funziona.</t>
+  </si>
+  <si>
+    <t>0.0 (?)</t>
+  </si>
+  <si>
+    <t>+0.25</t>
+  </si>
+  <si>
+    <t>TEORICAMENTE questa frase dovrebbe risultare inclusiva secondo le regole</t>
+  </si>
+  <si>
+    <t>non triggera alcuna regola anche se non è inclusivo perché bisognerebbe usare il dependency parser</t>
+  </si>
+  <si>
+    <t>ci vorrebbe il dependency parser</t>
+  </si>
+  <si>
+    <t>dovrebbe triggerare la regola</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>(mette prima il femminile)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> il det del primo il è uguale a advmod</t>
+  </si>
+  <si>
+    <t>-0.50</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -372,7 +420,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -550,6 +598,24 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -713,11 +779,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1072,484 +1144,748 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B63"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="135" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B25" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B28" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B29" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="144" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B31" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B32" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" s="6"/>
+    </row>
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B31" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B33" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B32" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="B35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B34" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B36" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B35" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" ht="120" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B38" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B39" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B38" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="105" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B39" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="B41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
+      <c r="B42" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B43" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B42" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="B44" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B43" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B46" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B45" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B47" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B46" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="B48" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B47" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="B49" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="B50" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B49" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="B52" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B51" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="C52" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B52" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B53" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="B54" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="B55" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C55" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B55" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
+      <c r="B56" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B56" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="B57" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B57" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B58" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B59" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
+      <c r="B60" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C60" s="7"/>
+    </row>
+    <row r="61" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B60" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="B61" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B61" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B62" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="B63" t="s">
-        <v>21</v>
+      <c r="B63" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>